<commit_message>
adding Operator related code
</commit_message>
<xml_diff>
--- a/documents/Learning Progress.xlsx
+++ b/documents/Learning Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vragawade\Documents\GitHub\Core-JAVA-Programming\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8423873A-97CE-4519-A202-8758DB5FBE9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2846DD-6DBC-423A-B218-0F6F2DA2151E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>Topics</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Current Progress</t>
+  </si>
+  <si>
+    <t>Delay</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +224,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -396,6 +405,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,8 +692,8 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -826,8 +838,8 @@
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="12" t="s">
-        <v>35</v>
+      <c r="H6" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -849,7 +861,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="5"/>
       <c r="H7" s="11" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -870,8 +882,8 @@
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="11" t="s">
-        <v>36</v>
+      <c r="H8" s="12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -890,7 +902,7 @@
       <c r="E9" s="32"/>
       <c r="F9" s="22"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -910,7 +922,7 @@
       <c r="E10" s="33"/>
       <c r="F10" s="23"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -932,7 +944,7 @@
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -954,7 +966,7 @@
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -976,7 +988,7 @@
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -998,7 +1010,7 @@
       </c>
       <c r="F14" s="24"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1018,7 +1030,7 @@
       <c r="E15" s="35"/>
       <c r="F15" s="25"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1038,7 +1050,7 @@
       <c r="E16" s="36"/>
       <c r="F16" s="26"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1060,7 +1072,7 @@
       </c>
       <c r="F17" s="24"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1080,7 +1092,7 @@
       <c r="E18" s="36"/>
       <c r="F18" s="26"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1102,7 +1114,7 @@
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1122,7 +1134,7 @@
       <c r="E20" s="38"/>
       <c r="F20" s="18"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1144,7 +1156,7 @@
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1164,7 +1176,7 @@
       <c r="E22" s="38"/>
       <c r="F22" s="18"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1186,7 +1198,7 @@
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="7"/>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1208,7 +1220,7 @@
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1230,7 +1242,7 @@
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1252,7 +1264,7 @@
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="11" t="s">
+      <c r="H26" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1274,7 +1286,7 @@
       </c>
       <c r="F27" s="27"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1294,7 +1306,7 @@
       <c r="E28" s="30"/>
       <c r="F28" s="28"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="11" t="s">
+      <c r="H28" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1316,7 +1328,7 @@
       </c>
       <c r="F29" s="16"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1338,7 +1350,7 @@
       </c>
       <c r="F30" s="16"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="11" t="s">
+      <c r="H30" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1360,7 +1372,7 @@
       </c>
       <c r="F31" s="16"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="11" t="s">
+      <c r="H31" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1382,7 +1394,7 @@
       </c>
       <c r="F32" s="16"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="39" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>